<commit_message>
multiple runs, changed prompt
</commit_message>
<xml_diff>
--- a/Analyses/part_III/data/LeidenAlgorithm_hypotheses.xlsx
+++ b/Analyses/part_III/data/LeidenAlgorithm_hypotheses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\Article_BasalAttributes\Analyses\part_III\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9340C129-0A5B-421D-923B-C4FF6697200F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B889E9-39F8-463A-B1A0-0019929A0496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>